<commit_message>
Update Care Provider and National Gini
</commit_message>
<xml_diff>
--- a/zzz_lib/code and data/app_data/metric_tables.xlsx
+++ b/zzz_lib/code and data/app_data/metric_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9eaf80618f9c5e5a/Work Items/TheCareBoard/zzz_lib/code and data/app_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07671965-672A-4B7C-B12C-7585E0221F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{07671965-672A-4B7C-B12C-7585E0221F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDB74FD5-696E-4664-ABF0-DE0EA37DC25E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2370" windowWidth="29040" windowHeight="15720" xr2:uid="{692BF238-EB5D-4EA1-B60C-5C9888F127F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{692BF238-EB5D-4EA1-B60C-5C9888F127F8}"/>
   </bookViews>
   <sheets>
     <sheet name="metric" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>page</t>
   </si>
   <si>
-    <t>Sandwich Generation Population</t>
-  </si>
-  <si>
     <t>{}</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
   </si>
   <si>
     <t>{0,1}</t>
-  </si>
-  <si>
-    <t>Daily Caregiving Hours</t>
   </si>
   <si>
     <t>sandwich-time</t>
@@ -306,6 +300,12 @@
   </si>
   <si>
     <t>2023 ACS 5-Year Estimates, Table B18101 &amp; Table S0101, US Census Bureau; 2024 CPS ASEC &amp; 5-year pooled ATUS (2018-2023, excluding 2020), US Census Bureau via IPUMS; 2024 Quarterly Census of Employment and Wages</t>
+  </si>
+  <si>
+    <t>Sandwich Generation: Population</t>
+  </si>
+  <si>
+    <t>Sandwich Generation: Daily Caregiving Hours</t>
   </si>
 </sst>
 </file>
@@ -716,15 +716,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0009D36D-AEED-4632-A201-2F17FDFE033D}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="174" style="5" bestFit="1" customWidth="1"/>
@@ -767,7 +767,7 @@
     </row>
     <row r="2" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -776,10 +776,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>2</v>
@@ -794,33 +794,33 @@
         <v>1</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>4</v>
@@ -829,290 +829,290 @@
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="I4" s="5">
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" s="5">
         <v>1</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="I6" s="5">
         <v>0</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="I7" s="5">
         <v>1</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="5">
         <v>0</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="5">
         <v>1</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="5">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="5">
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1196,7 +1196,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -1210,7 +1210,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Create updated care force without NAs
</commit_message>
<xml_diff>
--- a/zzz_lib/code and data/app_data/metric_tables.xlsx
+++ b/zzz_lib/code and data/app_data/metric_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9eaf80618f9c5e5a/Work Items/TheCareBoard/zzz_lib/code and data/app_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{07671965-672A-4B7C-B12C-7585E0221F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45A38A3-C429-4051-8D72-A50BE9B2F1EE}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{07671965-672A-4B7C-B12C-7585E0221F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1DF35AC-F96F-4BC4-926E-CE642AAE8478}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{692BF238-EB5D-4EA1-B60C-5C9888F127F8}"/>
   </bookViews>
@@ -195,12 +195,6 @@
     <t>Informal Care Force Participation</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;Formal Economic Value of Care&lt;/b&gt; estimates the total annual economic contribution of formal care work by aggregating the salaries of all formal care workers. </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Informal Economic Value of Care&lt;/b&gt; estimates the total annual economic contribution of unpaid care work by multiplying the total hours spent in informal care activities by the federal minimum wage. This is a lower-bound estimate of the value of informal care.</t>
-  </si>
-  <si>
     <t>Working-age adults caring for a child and an elderly adult.</t>
   </si>
   <si>
@@ -250,15 +244,9 @@
 A Care Ratio of one means there is one caregiver for every person in need. A ratio below one indicates a higher number of people in need of care for each available provider. A ratio above one is a higher number of people available to provide care than those needing care.</t>
   </si>
   <si>
-    <t>&lt;b&gt;The Informal Care Force Participation&lt;/b&gt; metric tracks the share of the total population (aged 18 and over) engaged in at least 3 hours of informal, unpaid care work in a day.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;The Sandwich Generation Population&lt;/b&gt; tracks the number of adults balancing the responsibilities of caring for both a child under 10 and an elderly adult.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;The Formal Care Force Participation&lt;/b&gt; metric tracks the share of the total population (aged 18 and over) employed in formal care occupations among all those working or looking for work. </t>
-  </si>
-  <si>
     <t>per day</t>
   </si>
   <si>
@@ -268,12 +256,6 @@
     <t>in informal care force</t>
   </si>
   <si>
-    <t>&lt;b&gt;Formal Care Hours Worked&lt;/b&gt; refers to the total hours worked in a day in paid care jobs by the entire U.S. population (aged 18 and over), also shown as the share of all formal hours worked in a day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;Informal Care Hours Worked&lt;/b&gt; refers to the total hours worked in unpaid care activities in a day by the entire U.S. population (aged 18 and over), also shown as the share of all informal hours worked in a day. </t>
-  </si>
-  <si>
     <t>Care Force</t>
   </si>
   <si>
@@ -305,6 +287,24 @@
   </si>
   <si>
     <t>The &lt;b&gt;Gini Coefficient of Formal Care&lt;/b&gt; measures how formal care jobs are geographically distributed across the U.S. among those individuals at risk of needing care. A Gini Coefficient of 0 would indicate perfect equality, meaning formal care jobs are evenly located in areas where at-risk individuals reside. A higher Gini Coefficient signals a greater mismatch in the availability of care by location. A Gini Coefficient usually measures income inequality, but here we use it to measure spatial inequality of care services to the population most at-risk of needing those services.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;The Informal Care Force Participation&lt;/b&gt; metric tracks the share of the total population (aged 18 and over) engaged in at least 3 hours of informal, unpaid care work in a day. &lt;b&gt;pp = percentage point&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Informal Care Hours Worked&lt;/b&gt; refers to the total hours worked in unpaid care activities in a day by the entire U.S. population (aged 18 and over), also shown as the share of all informal hours worked in a day. &lt;b&gt;pp = percentage point&lt;/b&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Formal Economic Value of Care&lt;/b&gt; estimates the total annual economic contribution of formal care work by aggregating the salaries of all formal care workers. &lt;b&gt;pp = percentage point&lt;/b&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Informal Economic Value of Care&lt;/b&gt; estimates the total annual economic contribution of unpaid care work by multiplying the total hours spent in informal care activities by the federal minimum wage. This is a lower-bound estimate of the value of informal care. &lt;b&gt;pp = percentage point&lt;/b&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Formal Care Hours Worked&lt;/b&gt; refers to the total hours worked in a day in paid care jobs by the entire U.S. population (aged 18 and over), also shown as the share of all formal hours worked in a day. &lt;b&gt;pp = percentage point&lt;/b&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;The Formal Care Force Participation&lt;/b&gt; metric tracks the share of the total population (aged 18 and over) employed in formal care occupations among all those working or looking for work. &lt;b&gt;pp = percentage point&lt;/b&gt; </t>
   </si>
 </sst>
 </file>
@@ -394,6 +394,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -715,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0009D36D-AEED-4632-A201-2F17FDFE033D}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,10 +779,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>2</v>
@@ -793,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="225" x14ac:dyDescent="0.25">
@@ -807,16 +811,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>38</v>
@@ -828,10 +832,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -842,13 +846,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
@@ -863,24 +867,24 @@
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>32</v>
@@ -898,10 +902,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -915,10 +919,10 @@
         <v>49</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>27</v>
@@ -933,13 +937,13 @@
         <v>0</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
@@ -950,10 +954,10 @@
         <v>50</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>27</v>
@@ -968,13 +972,13 @@
         <v>1</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
@@ -985,7 +989,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>32</v>
@@ -994,7 +998,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>29</v>
@@ -1003,13 +1007,13 @@
         <v>0</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -1020,7 +1024,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>32</v>
@@ -1029,7 +1033,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>29</v>
@@ -1038,10 +1042,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1055,10 +1059,10 @@
         <v>33</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>27</v>
@@ -1073,13 +1077,13 @@
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
@@ -1090,10 +1094,10 @@
         <v>35</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>27</v>
@@ -1108,10 +1112,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1178,7 +1182,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1209,7 +1213,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>

</xml_diff>